<commit_message>
Recreated integration test excel file
Ticket: #200
Change-Id: I15af718adc99d7dd26d77201c68e1afc391ff6d9
</commit_message>
<xml_diff>
--- a/test/data/mps155_timezone_bug_validated.xlsx
+++ b/test/data/mps155_timezone_bug_validated.xlsx
@@ -204,6 +204,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t>Matrix</t>
     </r>
     <r>
@@ -226,6 +227,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probe-nahme
 </t>
     </r>
@@ -240,6 +242,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probe-nahme
 </t>
     </r>
@@ -326,6 +329,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">b) Verwenden Sie bitte für jeden Erreger (getrennt auch für VTEC und kommensale </t>
     </r>
     <r>
@@ -354,6 +358,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t>Probenummer nach der "Allgemeinen Verwaltungsvorschrift über den Austausch von Daten im Bereich der Lebensmittelsicherheit und des Verbraucherschutzes" (AVVData), die an das BVL übermittelt wird.</t>
     </r>
     <r>
@@ -440,6 +445,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Erreger
 </t>
     </r>
@@ -460,6 +466,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">ADV-Code angeben
 </t>
     </r>
@@ -484,6 +491,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Kodiersystem mit
 Matrix-Code angeben
 (ADV2 + ADV3)
@@ -510,6 +518,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">ADV-Code angeben
 </t>
     </r>
@@ -571,6 +580,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probe-nahme
 </t>
     </r>
@@ -585,6 +595,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Matrix
 Code
 </t>
@@ -600,6 +611,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Oberbegriff (Kodier-system) der Matrizes
 </t>
     </r>
@@ -614,6 +626,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Grund der Probe-nahme
 </t>
     </r>
@@ -628,6 +641,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Betriebsart
 </t>
     </r>
@@ -645,6 +659,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ver-arbeitungs-zustand
 </t>
     </r>
@@ -659,6 +674,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Bemerkung
 </t>
     </r>
@@ -682,6 +698,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Betriebsart
 </t>
     </r>
@@ -696,6 +713,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Untersuchungsauftrag für Isolate/Proben </t>
     </r>
     <r>
@@ -711,6 +729,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Grund der Probe-nahme
 </t>
     </r>
@@ -725,6 +744,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probenahme (ADV-Kat.Nr. 9) </t>
     </r>
     <r>
@@ -740,6 +760,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Oberbegriff (Kodiersystem) der Matrizes (ADV-Kat-Nr. 2) </t>
     </r>
     <r>
@@ -755,6 +776,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Matrix-Code (ADV-Kat.Nr. 3) </t>
     </r>
     <r>
@@ -770,6 +792,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Verarbeitungszustand (ADV-Kat-Nr.12) </t>
     </r>
     <r>
@@ -785,6 +808,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Grund der Probenahme (ADV-Kat.Nr. 4) </t>
     </r>
     <r>
@@ -800,6 +824,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Betriebsart (ADV-Kat-Nr.8) </t>
     </r>
     <r>
@@ -833,6 +858,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Erreger
 </t>
     </r>
@@ -847,6 +873,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t>Z.B. Zoonosen-Stichprobenplan-</t>
     </r>
     <r>
@@ -903,6 +930,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Erreger
 </t>
     </r>
@@ -917,6 +945,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Erreger
 </t>
     </r>
@@ -931,6 +960,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probe-nahme
 </t>
     </r>
@@ -945,6 +975,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probe-nahme
 </t>
     </r>
@@ -959,6 +990,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ort der Probe-nahme
 </t>
     </r>
@@ -973,6 +1005,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Oberbe-griff (Kodier-system) der Matrizes
 </t>
     </r>
@@ -987,6 +1020,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Matrix
 Code
 </t>
@@ -1002,6 +1036,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Matrix
 </t>
     </r>
@@ -1016,6 +1051,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Ver-arbeitungs-zustand
 </t>
     </r>
@@ -1030,6 +1066,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Grund der Probe-nahme
 </t>
     </r>
@@ -1044,6 +1081,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Grund der Probe-nahme
 </t>
     </r>
@@ -1058,6 +1096,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Betriebsart
 </t>
     </r>
@@ -1072,6 +1111,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Betriebsart
 </t>
     </r>
@@ -1086,6 +1126,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Bemerkung
 </t>
     </r>
@@ -1100,6 +1141,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Bitte senden Sie die Excel-Datei mit eindeutiger Zuordnung (z.B. "E.coli.xlsx") an die allgemeine E-Mail-Adresse der mikrobiologischen NRLs des BfR: </t>
     </r>
     <r>
@@ -1122,6 +1164,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Weitergehende molekularbiologische Feintypisierung </t>
     </r>
     <r>
@@ -1136,6 +1179,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Vergleiche mit humanen Isolaten </t>
     </r>
     <r>
@@ -1156,6 +1200,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">Bitte führen Sie folgende Untersuchungen der Isolate durch </t>
     </r>
     <r>
@@ -1185,6 +1230,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">NRL </t>
     </r>
     <r>
@@ -1219,6 +1265,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">- Escherichia coli
 - Escherichia coli ESBL-bildend
 - Escherichia coli AmpC-bildend
@@ -1249,6 +1296,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">    </t>
     </r>
     <r>
@@ -1353,6 +1401,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">    </t>
     </r>
     <r>
@@ -1419,6 +1468,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t>(x)</t>
     </r>
     <r>
@@ -1437,6 +1487,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">f) Die ADV-Codes (Codes zur </t>
     </r>
     <r>
@@ -1514,6 +1565,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t>a) Für die Sicherung der ordnungsgemäßen Abläufe und Dokumentation der Probenahme und den Versand von Probenmaterial ist der Einsender verantwortlich. Besondere Hinweise z.B. zum Zustand von Proben oder besonderer Sicherheitshinweise hinterlegen Sie bitte im Bemerkungsfeld. Bitte beachten Sie auch das Dokument "Allgemeine Bedingungen für den Austausch von Materialien - Vergabe an das BfR ", welches Sie auf der Internetseite des BfR (</t>
     </r>
     <r>
@@ -1546,6 +1598,7 @@
   </si>
   <si>
     <r>
+      <rPr/>
       <t xml:space="preserve">ADV-Code aus Katalog-Nr. 12; z. B. 051 = mit Haut oder 040 = unverarbeitet/roh; ggf. </t>
     </r>
     <r>
@@ -1593,10 +1646,317 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Untersuchungsauftrag für Isolate/Proben </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>a,b</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve"/>
   </si>
   <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Bitte führen Sie folgende Untersuchungen der Isolate durch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>c</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Weitergehende molekularbiologische Feintypisierung </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Vergleiche mit humanen Isolaten </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>e</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Bitte senden Sie die Excel-Datei mit eindeutiger Zuordnung (z.B. "E.coli.xlsx") an die allgemeine E-Mail-Adresse der mikrobiologischen NRLs des BfR: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>NRLs-Mibi@bfr.bund.de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Erreger
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Text aus ADV-Kat-Nr.16)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Erreger
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.9)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(PLZ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Text)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Oberbe-griff (Kodier-system) der Matrizes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Matrix
+Code
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Matrix
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ver-arbeitungs-zustand
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.12)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Grund der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Grund der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Betriebsart
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.8)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Betriebsart
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Bemerkung
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(u.a. Untersuchungs-programm)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -1756,6 +2116,837 @@
   </si>
   <si>
     <t xml:space="preserve">8000000</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>Probenummer nach der "Allgemeinen Verwaltungsvorschrift über den Austausch von Daten im Bereich der Lebensmittelsicherheit und des Verbraucherschutzes" (AVVData), die an das BVL übermittelt wird.</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probenahme (ADV-Kat.Nr. 9) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">ADV-Code angeben
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>oder / und</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+PLZ mit Ort angeben</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Oberbegriff (Kodiersystem) der Matrizes (ADV-Kat-Nr. 2) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Kodiersystem mit
+Matrix-Code angeben
+(ADV2 + ADV3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>oder / und</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Matrix als Text angeben</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Matrix-Code (ADV-Kat.Nr. 3) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Verarbeitungszustand (ADV-Kat-Nr.12) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">ADV-Code aus Katalog-Nr. 12; z. B. 051 = mit Haut oder 040 = unverarbeitet/roh; ggf. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pflicht</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, wenn Betriebsart mit 4 beginnt / es den Einzelhandel betrifft</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>(x)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> g</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Grund der Probenahme (ADV-Kat.Nr. 4) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">ADV-Code angeben
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">oder / und </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Text</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Betriebsart (ADV-Kat-Nr.8) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>f</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>Z.B. Zoonosen-Stichprobenplan-</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Programm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> oder </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>geografische Herkunft</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> der Probe; bitte ggf. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>epidemiologisch relevante Daten</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> angeben (z.B. Ausbruch in einem Bestand; Isolate im Zusammenhang mit Erkrankungen von Personen - auch vermutet: ja/nein)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Erreger
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Text aus ADV-Kat-Nr.16)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Erreger
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.9)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(PLZ)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ort der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Text)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Oberbegriff (Kodier-system) der Matrizes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Matrix
+Code
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>Matrix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Ver-arbeitungs-zustand
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.12)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Grund der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.4)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Grund der Probe-nahme
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Betriebsart
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Code aus ADV-Kat-Nr.8)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Betriebsart
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(Textfeld/ Ergänzung)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Bemerkung
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="6.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(u.a. Untersuchungs-programm)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t>a) Für die Sicherung der ordnungsgemäßen Abläufe und Dokumentation der Probenahme und den Versand von Probenmaterial ist der Einsender verantwortlich. Besondere Hinweise z.B. zum Zustand von Proben oder besonderer Sicherheitshinweise hinterlegen Sie bitte im Bemerkungsfeld. Bitte beachten Sie auch das Dokument "Allgemeine Bedingungen für den Austausch von Materialien - Vergabe an das BfR ", welches Sie auf der Internetseite des BfR (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.bfr.bund.de/cm/343/mt-bedingungen-teil-b.pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) finden können.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">b) Verwenden Sie bitte für jeden Erreger (getrennt auch für VTEC und kommensale </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>E. coli</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sowie MRSA und andere Staphylokokken) einen separaten Einsendebogen.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">f) Die ADV-Codes (Codes zur </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">utomatisierten </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aten</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>erarbeitung) finden Sie auf der Homepage des Bundesamtes für Verbraucherschutz und Lebensmittelsicherheit (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="3"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>http://www.bvl.bund.de</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>). Bitte verwenden Sie stets den vollständigen Code.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">NRL </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>E. coli</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">- Escherichia coli
+- Escherichia coli ESBL-bildend
+- Escherichia coli AmpC-bildend
+- Escherichia coli ESBL/AmpC-bildend
+- Escherichia coli Carbapenemase-bildend
+- Genus Enterococcus
+- Enterococcus faecalis
+- Enterococcus faecium
+- [Andere </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Carbapenemase-bildende</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Enterobacteriaceae (z.B. Klebsiella, Enterobacter, Citrobacter…)]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ADV-Code angeben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+        oder / und </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Beispiele:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ZoMo-Bek
+- VO 2073</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- 81 bzw. Zoonosen-Monitoring - Planprobe bzw. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ZoMo-Nat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> bzw. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ZSP</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ADV-Code angeben</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+        oder / und </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Beispiele:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>- Diagnostik
+- 81 bzw. Zoonosen-Monitoring - Planprobe</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -8666,7 +9857,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="21">
       <c r="A1" t="s" s="221">
-        <v>148</v>
+        <v>208</v>
       </c>
       <c r="B1" s="222"/>
       <c r="C1" s="222"/>
@@ -8821,7 +10012,7 @@
         <v>87</v>
       </c>
       <c r="B7" t="s" s="226">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" s="226"/>
       <c r="D7" s="226"/>
@@ -8933,7 +10124,7 @@
       <c r="H11" s="140"/>
       <c r="I11" s="140"/>
       <c r="J11" t="s" s="149">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="K11" s="150"/>
       <c r="L11" s="151"/>
@@ -8954,7 +10145,7 @@
       </c>
       <c r="B12" s="225"/>
       <c r="C12" t="s" s="227">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D12" s="227"/>
       <c r="E12" s="227"/>
@@ -8971,7 +10162,7 @@
       <c r="N12" s="238"/>
       <c r="O12" s="239"/>
       <c r="P12" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q12" s="153"/>
       <c r="R12" s="153"/>
@@ -8999,7 +10190,7 @@
       <c r="N13" s="232"/>
       <c r="O13" s="233"/>
       <c r="P13" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q13" s="153"/>
       <c r="R13" s="153"/>
@@ -9040,7 +10231,7 @@
       </c>
       <c r="B15" s="220"/>
       <c r="C15" t="s" s="227">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D15" s="227"/>
       <c r="E15" s="227"/>
@@ -9057,7 +10248,7 @@
       <c r="N15" s="235"/>
       <c r="O15" s="236"/>
       <c r="P15" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q15" s="153"/>
       <c r="R15" s="153"/>
@@ -9085,7 +10276,7 @@
       <c r="N16" s="235"/>
       <c r="O16" s="236"/>
       <c r="P16" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q16" s="153"/>
       <c r="R16" s="153"/>
@@ -9100,7 +10291,7 @@
       </c>
       <c r="B17" s="220"/>
       <c r="C17" t="s" s="227">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D17" s="227"/>
       <c r="E17" s="227"/>
@@ -9109,7 +10300,7 @@
       <c r="H17" s="227"/>
       <c r="I17" s="168"/>
       <c r="J17" t="s" s="234">
-        <v>179</v>
+        <v>211</v>
       </c>
       <c r="K17" s="235"/>
       <c r="L17" s="235"/>
@@ -9117,7 +10308,7 @@
       <c r="N17" s="235"/>
       <c r="O17" s="236"/>
       <c r="P17" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q17" s="153"/>
       <c r="R17" s="153"/>
@@ -9145,7 +10336,7 @@
       <c r="N18" s="232"/>
       <c r="O18" s="233"/>
       <c r="P18" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q18" s="153"/>
       <c r="R18" s="153"/>
@@ -9158,7 +10349,7 @@
       </c>
       <c r="B19" s="220"/>
       <c r="C19" t="s" s="227">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D19" s="227"/>
       <c r="E19" s="227"/>
@@ -9186,7 +10377,7 @@
       </c>
       <c r="B20" s="220"/>
       <c r="C20" t="s" s="227">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D20" s="227"/>
       <c r="E20" s="227"/>
@@ -9203,7 +10394,7 @@
       <c r="N20" s="232"/>
       <c r="O20" s="233"/>
       <c r="P20" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q20" s="153"/>
       <c r="R20" s="153"/>
@@ -9218,7 +10409,7 @@
       </c>
       <c r="B21" s="220"/>
       <c r="C21" t="s" s="227">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D21" s="227"/>
       <c r="E21" s="227"/>
@@ -9235,7 +10426,7 @@
       <c r="N21" s="232"/>
       <c r="O21" s="233"/>
       <c r="P21" t="s" s="137">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q21" s="153"/>
       <c r="R21" s="153"/>
@@ -9250,7 +10441,7 @@
       </c>
       <c r="B22" s="220"/>
       <c r="C22" t="s" s="227">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D22" s="227"/>
       <c r="E22" s="227"/>
@@ -9259,7 +10450,7 @@
       <c r="H22" s="227"/>
       <c r="I22" s="168"/>
       <c r="J22" t="s" s="228">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K22" s="229"/>
       <c r="L22" s="229"/>
@@ -9285,7 +10476,7 @@
       <c r="H23" s="140"/>
       <c r="I23" s="140"/>
       <c r="J23" t="s" s="228">
-        <v>180</v>
+        <v>213</v>
       </c>
       <c r="K23" s="229"/>
       <c r="L23" s="229"/>
@@ -9293,7 +10484,7 @@
       <c r="N23" s="229"/>
       <c r="O23" s="230"/>
       <c r="P23" t="s" s="138">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q23" s="153"/>
       <c r="R23" s="153"/>
@@ -9310,7 +10501,7 @@
       <c r="H24" s="140"/>
       <c r="I24" s="140"/>
       <c r="J24" t="s" s="228">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="K24" s="229"/>
       <c r="L24" s="229"/>
@@ -9564,7 +10755,7 @@
     </row>
     <row r="36" spans="1:25" s="127" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A36" t="s" s="146">
-        <v>178</v>
+        <v>214</v>
       </c>
       <c r="B36" s="140"/>
       <c r="C36" s="140"/>
@@ -9689,10 +10880,10 @@
         <v>53</v>
       </c>
       <c r="C41" t="s" s="111">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="D41" t="s" s="112">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="E41" t="s" s="113">
         <v>73</v>
@@ -9701,69 +10892,69 @@
         <v>1</v>
       </c>
       <c r="G41" t="s" s="111">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="H41" t="s" s="115">
-        <v>167</v>
+        <v>218</v>
       </c>
       <c r="I41" t="s" s="112">
-        <v>168</v>
+        <v>219</v>
       </c>
       <c r="J41" t="s" s="113">
-        <v>169</v>
+        <v>220</v>
       </c>
       <c r="K41" t="s" s="115">
-        <v>170</v>
+        <v>221</v>
       </c>
       <c r="L41" t="s" s="114">
-        <v>171</v>
+        <v>222</v>
       </c>
       <c r="M41" t="s" s="116">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="N41" t="s" s="113">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="O41" t="s" s="114">
-        <v>174</v>
+        <v>225</v>
       </c>
       <c r="P41" t="s" s="111">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="Q41" t="s" s="112">
-        <v>176</v>
+        <v>227</v>
       </c>
       <c r="R41" t="s" s="116">
         <v>144</v>
       </c>
       <c r="S41" t="s" s="116">
-        <v>177</v>
+        <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:25" s="77" customFormat="1" ht="21.75" customHeight="1">
       <c r="A42" t="s" s="315">
-        <v>210</v>
+        <v>229</v>
       </c>
       <c r="B42" t="s" s="316">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="C42" t="s" s="317">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="D42" t="s" s="318">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E42" t="s" s="319">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="F42" t="s" s="320">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="G42" t="s" s="321">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="H42" t="s" s="322">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="I42" t="s" s="323">
         <v>54</v>
@@ -9772,58 +10963,58 @@
         <v>89</v>
       </c>
       <c r="K42" t="s" s="325">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="L42" t="s" s="326">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="M42" t="s" s="327">
-        <v>219</v>
+        <v>238</v>
       </c>
       <c r="N42" t="s" s="328">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="O42" t="s" s="329">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="P42" t="s" s="330">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="Q42" t="s" s="331">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="R42" t="s" s="332">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S42" t="s" s="333">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="T42" s="334"/>
     </row>
     <row r="43" spans="1:25" s="10" customFormat="1" ht="21.75" customHeight="1">
       <c r="A43" t="s" s="335">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B43" t="s" s="336">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C43" t="s" s="337">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="D43" t="s" s="338">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="E43" t="s" s="339">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="F43" t="s" s="340">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="G43" t="s" s="341">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="H43" t="s" s="342">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="I43" t="s" s="343">
         <v>54</v>
@@ -9832,118 +11023,118 @@
         <v>89</v>
       </c>
       <c r="K43" t="s" s="345">
-        <v>217</v>
+        <v>236</v>
       </c>
       <c r="L43" t="s" s="346">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="M43" t="s" s="347">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="N43" t="s" s="348">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="O43" t="s" s="349">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="P43" t="s" s="350">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="Q43" t="s" s="351">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="R43" t="s" s="352">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S43" t="s" s="353">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="T43" s="354"/>
     </row>
     <row r="44" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
       <c r="A44" t="s" s="355">
-        <v>226</v>
+        <v>245</v>
       </c>
       <c r="B44" t="s" s="356">
-        <v>227</v>
+        <v>246</v>
       </c>
       <c r="C44" t="s" s="357">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="D44" t="s" s="358">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E44" t="s" s="359">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="F44" t="s" s="360">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="G44" t="s" s="361">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H44" t="s" s="362">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="I44" t="s" s="363">
         <v>54</v>
       </c>
       <c r="J44" t="s" s="364">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="K44" t="s" s="365">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="L44" t="s" s="366">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="M44" t="s" s="367">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N44" t="s" s="368">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O44" t="s" s="369">
         <v>124</v>
       </c>
       <c r="P44" t="s" s="370">
+        <v>253</v>
+      </c>
+      <c r="Q44" t="s" s="371">
+        <v>254</v>
+      </c>
+      <c r="R44" t="s" s="372">
+        <v>209</v>
+      </c>
+      <c r="S44" t="s" s="373">
+        <v>255</v>
+      </c>
+      <c r="T44" s="374"/>
+    </row>
+    <row r="45" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A45" t="s" s="375">
+        <v>256</v>
+      </c>
+      <c r="B45" t="s" s="376">
+        <v>257</v>
+      </c>
+      <c r="C45" t="s" s="377">
+        <v>258</v>
+      </c>
+      <c r="D45" t="s" s="378">
+        <v>209</v>
+      </c>
+      <c r="E45" t="s" s="379">
+        <v>259</v>
+      </c>
+      <c r="F45" t="s" s="380">
+        <v>260</v>
+      </c>
+      <c r="G45" t="s" s="381">
         <v>234</v>
       </c>
-      <c r="Q44" t="s" s="371">
+      <c r="H45" t="s" s="382">
         <v>235</v>
-      </c>
-      <c r="R44" t="s" s="372">
-        <v>208</v>
-      </c>
-      <c r="S44" t="s" s="373">
-        <v>236</v>
-      </c>
-      <c r="T44" s="374"/>
-    </row>
-    <row r="45" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A45" t="s" s="375">
-        <v>237</v>
-      </c>
-      <c r="B45" t="s" s="376">
-        <v>238</v>
-      </c>
-      <c r="C45" t="s" s="377">
-        <v>239</v>
-      </c>
-      <c r="D45" t="s" s="378">
-        <v>208</v>
-      </c>
-      <c r="E45" t="s" s="379">
-        <v>240</v>
-      </c>
-      <c r="F45" t="s" s="380">
-        <v>241</v>
-      </c>
-      <c r="G45" t="s" s="381">
-        <v>215</v>
-      </c>
-      <c r="H45" t="s" s="382">
-        <v>216</v>
       </c>
       <c r="I45" t="s" s="383">
         <v>54</v>
@@ -9952,211 +11143,211 @@
         <v>89</v>
       </c>
       <c r="K45" t="s" s="385">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="L45" t="s" s="386">
-        <v>243</v>
+        <v>262</v>
       </c>
       <c r="M45" t="s" s="387">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="N45" t="s" s="388">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="O45" t="s" s="389">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P45" t="s" s="390">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="Q45" t="s" s="391">
-        <v>244</v>
+        <v>263</v>
       </c>
       <c r="R45" t="s" s="392">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S45" t="s" s="393">
-        <v>245</v>
+        <v>264</v>
       </c>
       <c r="T45" s="394"/>
     </row>
     <row r="46" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
       <c r="A46" t="s" s="395">
-        <v>246</v>
+        <v>265</v>
       </c>
       <c r="B46" t="s" s="396">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="C46" t="s" s="397">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="D46" t="s" s="398">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E46" t="s" s="399">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="F46" t="s" s="400">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="G46" t="s" s="401">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="H46" t="s" s="402">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="I46" t="s" s="403">
         <v>54</v>
       </c>
       <c r="J46" t="s" s="404">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="K46" t="s" s="405">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="L46" t="s" s="406">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="M46" t="s" s="407">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N46" t="s" s="408">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="O46" t="s" s="409">
         <v>124</v>
       </c>
       <c r="P46" t="s" s="410">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="Q46" t="s" s="411">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R46" t="s" s="412">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="S46" t="s" s="413">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="T46" s="414"/>
     </row>
     <row r="47" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
       <c r="A47" t="s" s="415">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="B47" t="s" s="416">
-        <v>254</v>
+        <v>273</v>
       </c>
       <c r="C47" t="s" s="417">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="D47" t="s" s="418">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E47" t="s" s="419">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="F47" t="s" s="420">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="G47" t="s" s="421">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="H47" t="s" s="422">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="I47" t="s" s="423">
         <v>54</v>
       </c>
       <c r="J47" t="s" s="424">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="K47" t="s" s="425">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="L47" t="s" s="426">
-        <v>233</v>
+        <v>252</v>
       </c>
       <c r="M47" t="s" s="427">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N47" t="s" s="428">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="O47" t="s" s="429">
         <v>124</v>
       </c>
       <c r="P47" t="s" s="430">
-        <v>251</v>
+        <v>270</v>
       </c>
       <c r="Q47" t="s" s="431">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R47" t="s" s="432">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="S47" t="s" s="433">
-        <v>236</v>
+        <v>255</v>
       </c>
       <c r="T47" s="434"/>
     </row>
     <row r="48" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
       <c r="A48" t="s" s="435">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="B48" t="s" s="436">
-        <v>258</v>
+        <v>277</v>
       </c>
       <c r="C48" t="s" s="437">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="D48" t="s" s="438">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E48" t="s" s="439">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="F48" t="s" s="440">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="G48" t="s" s="441">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="H48" t="s" s="442">
-        <v>216</v>
+        <v>235</v>
       </c>
       <c r="I48" t="s" s="443">
         <v>54</v>
       </c>
       <c r="J48" t="s" s="444">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="K48" t="s" s="445">
-        <v>260</v>
+        <v>279</v>
       </c>
       <c r="L48" t="s" s="446">
-        <v>261</v>
+        <v>280</v>
       </c>
       <c r="M48" t="s" s="447">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="N48" t="s" s="448">
-        <v>250</v>
+        <v>269</v>
       </c>
       <c r="O48" t="s" s="449">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="P48" t="s" s="450">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="Q48" t="s" s="451">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R48" t="s" s="452">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S48" t="s" s="453">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="T48" s="454"/>
     </row>
@@ -50113,7 +51304,7 @@
       <c r="C6" s="256"/>
       <c r="D6" s="256"/>
       <c r="E6" t="s" s="257">
-        <v>93</v>
+        <v>282</v>
       </c>
       <c r="F6" s="258"/>
       <c r="G6" s="258"/>
@@ -50260,7 +51451,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s" s="255">
-        <v>150</v>
+        <v>283</v>
       </c>
       <c r="C11" s="256"/>
       <c r="D11" s="256"/>
@@ -50281,7 +51472,7 @@
       <c r="Q11" s="243"/>
       <c r="R11" s="243"/>
       <c r="S11" t="s" s="243">
-        <v>121</v>
+        <v>284</v>
       </c>
       <c r="T11" s="244"/>
     </row>
@@ -50346,7 +51537,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s" s="268">
-        <v>151</v>
+        <v>285</v>
       </c>
       <c r="C14" s="256"/>
       <c r="D14" s="256"/>
@@ -50365,11 +51556,11 @@
       <c r="O14" s="258"/>
       <c r="P14" s="259"/>
       <c r="Q14" t="s" s="243">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="R14" s="243"/>
       <c r="S14" t="s" s="243">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="T14" s="244"/>
     </row>
@@ -50378,7 +51569,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s" s="255">
-        <v>152</v>
+        <v>287</v>
       </c>
       <c r="C15" s="256"/>
       <c r="D15" s="256"/>
@@ -50434,12 +51625,12 @@
         <v>25</v>
       </c>
       <c r="B17" t="s" s="255">
-        <v>153</v>
+        <v>288</v>
       </c>
       <c r="C17" s="255"/>
       <c r="D17" s="255"/>
       <c r="E17" t="s" s="257">
-        <v>204</v>
+        <v>289</v>
       </c>
       <c r="F17" s="258"/>
       <c r="G17" s="258"/>
@@ -50455,7 +51646,7 @@
       <c r="Q17" s="243"/>
       <c r="R17" s="243"/>
       <c r="S17" t="s" s="243">
-        <v>197</v>
+        <v>290</v>
       </c>
       <c r="T17" s="244"/>
     </row>
@@ -50464,7 +51655,7 @@
         <v>61</v>
       </c>
       <c r="B18" t="s" s="255">
-        <v>154</v>
+        <v>291</v>
       </c>
       <c r="C18" s="256"/>
       <c r="D18" s="256"/>
@@ -50485,7 +51676,7 @@
       <c r="Q18" s="243"/>
       <c r="R18" s="243"/>
       <c r="S18" t="s" s="243">
-        <v>123</v>
+        <v>292</v>
       </c>
       <c r="T18" s="244"/>
     </row>
@@ -50522,7 +51713,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s" s="255">
-        <v>155</v>
+        <v>293</v>
       </c>
       <c r="C20" s="256"/>
       <c r="D20" s="256"/>
@@ -50543,7 +51734,7 @@
       <c r="Q20" s="243"/>
       <c r="R20" s="243"/>
       <c r="S20" t="s" s="243">
-        <v>123</v>
+        <v>292</v>
       </c>
       <c r="T20" s="244"/>
     </row>
@@ -50601,7 +51792,7 @@
       <c r="Q22" s="243"/>
       <c r="R22" s="243"/>
       <c r="S22" t="s" s="243">
-        <v>197</v>
+        <v>290</v>
       </c>
       <c r="T22" s="244"/>
     </row>
@@ -50615,7 +51806,7 @@
       <c r="C23" s="263"/>
       <c r="D23" s="263"/>
       <c r="E23" t="s" s="251">
-        <v>163</v>
+        <v>294</v>
       </c>
       <c r="F23" s="252"/>
       <c r="G23" s="252"/>
@@ -50760,10 +51951,10 @@
         <v>53</v>
       </c>
       <c r="D29" t="s" s="27">
-        <v>118</v>
+        <v>295</v>
       </c>
       <c r="E29" t="s" s="28">
-        <v>162</v>
+        <v>296</v>
       </c>
       <c r="F29" t="s" s="7">
         <v>73</v>
@@ -50772,43 +51963,43 @@
         <v>1</v>
       </c>
       <c r="H29" t="s" s="27">
-        <v>136</v>
+        <v>297</v>
       </c>
       <c r="I29" t="s" s="8">
-        <v>64</v>
+        <v>298</v>
       </c>
       <c r="J29" t="s" s="28">
-        <v>65</v>
+        <v>299</v>
       </c>
       <c r="K29" t="s" s="7">
-        <v>138</v>
+        <v>300</v>
       </c>
       <c r="L29" t="s" s="8">
-        <v>137</v>
+        <v>301</v>
       </c>
       <c r="M29" t="s" s="9">
-        <v>60</v>
+        <v>302</v>
       </c>
       <c r="N29" t="s" s="29">
-        <v>142</v>
+        <v>303</v>
       </c>
       <c r="O29" t="s" s="7">
-        <v>139</v>
+        <v>304</v>
       </c>
       <c r="P29" t="s" s="9">
-        <v>149</v>
+        <v>305</v>
       </c>
       <c r="Q29" t="s" s="27">
-        <v>140</v>
+        <v>306</v>
       </c>
       <c r="R29" t="s" s="28">
-        <v>147</v>
+        <v>307</v>
       </c>
       <c r="S29" t="s" s="31">
         <v>96</v>
       </c>
       <c r="T29" t="s" s="30">
-        <v>143</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="33.75">
@@ -51039,7 +52230,7 @@
     </row>
     <row r="36" spans="1:20" s="72" customFormat="1" ht="24.75" customHeight="1">
       <c r="A36" t="s" s="254">
-        <v>200</v>
+        <v>309</v>
       </c>
       <c r="B36" s="254"/>
       <c r="C36" s="254"/>
@@ -51063,7 +52254,7 @@
     </row>
     <row r="37" spans="1:20" s="72" customFormat="1" ht="12.95" customHeight="1">
       <c r="A37" t="s" s="248">
-        <v>90</v>
+        <v>310</v>
       </c>
       <c r="B37" s="248"/>
       <c r="C37" s="248"/>
@@ -51159,7 +52350,7 @@
     </row>
     <row r="41" spans="1:20" s="72" customFormat="1" ht="12.95" customHeight="1">
       <c r="A41" t="s" s="248">
-        <v>199</v>
+        <v>311</v>
       </c>
       <c r="B41" s="248"/>
       <c r="C41" s="248"/>
@@ -51413,7 +52604,7 @@
       </c>
       <c r="R3" s="284"/>
       <c r="S3" t="s" s="280">
-        <v>185</v>
+        <v>312</v>
       </c>
       <c r="T3" s="284"/>
       <c r="U3" t="s" s="301">
@@ -51477,7 +52668,7 @@
       <c r="C5" s="256"/>
       <c r="D5" s="256"/>
       <c r="E5" t="s" s="257">
-        <v>93</v>
+        <v>282</v>
       </c>
       <c r="F5" s="258"/>
       <c r="G5" s="258"/>
@@ -51538,7 +52729,7 @@
       </c>
       <c r="V6" s="243"/>
       <c r="W6" t="s" s="297">
-        <v>192</v>
+        <v>313</v>
       </c>
       <c r="X6" s="304"/>
       <c r="Y6" s="183"/>
@@ -51655,7 +52846,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s" s="255">
-        <v>150</v>
+        <v>283</v>
       </c>
       <c r="C10" s="256"/>
       <c r="D10" s="256"/>
@@ -51676,11 +52867,11 @@
       <c r="Q10" s="243"/>
       <c r="R10" s="243"/>
       <c r="S10" t="s" s="243">
-        <v>121</v>
+        <v>284</v>
       </c>
       <c r="T10" s="243"/>
       <c r="U10" t="s" s="243">
-        <v>121</v>
+        <v>284</v>
       </c>
       <c r="V10" s="243"/>
       <c r="W10" s="243"/>
@@ -51758,7 +52949,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s" s="268">
-        <v>151</v>
+        <v>285</v>
       </c>
       <c r="C13" s="256"/>
       <c r="D13" s="256"/>
@@ -51777,19 +52968,19 @@
       <c r="O13" s="258"/>
       <c r="P13" s="259"/>
       <c r="Q13" t="s" s="243">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="R13" s="243"/>
       <c r="S13" t="s" s="243">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="T13" s="243"/>
       <c r="U13" t="s" s="243">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="V13" s="243"/>
       <c r="W13" t="s" s="243">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="X13" s="244"/>
       <c r="Y13" s="183"/>
@@ -51799,7 +52990,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s" s="255">
-        <v>152</v>
+        <v>287</v>
       </c>
       <c r="C14" s="256"/>
       <c r="D14" s="256"/>
@@ -51865,7 +53056,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s" s="255">
-        <v>153</v>
+        <v>288</v>
       </c>
       <c r="C16" s="255"/>
       <c r="D16" s="255"/>
@@ -51898,7 +53089,7 @@
         <v>61</v>
       </c>
       <c r="B17" t="s" s="255">
-        <v>154</v>
+        <v>291</v>
       </c>
       <c r="C17" s="256"/>
       <c r="D17" s="256"/>
@@ -51917,19 +53108,19 @@
       <c r="O17" s="258"/>
       <c r="P17" s="259"/>
       <c r="Q17" t="s" s="297">
-        <v>193</v>
+        <v>314</v>
       </c>
       <c r="R17" s="298"/>
       <c r="S17" t="s" s="243">
-        <v>123</v>
+        <v>292</v>
       </c>
       <c r="T17" s="243"/>
       <c r="U17" t="s" s="243">
-        <v>123</v>
+        <v>292</v>
       </c>
       <c r="V17" s="243"/>
       <c r="W17" t="s" s="297">
-        <v>194</v>
+        <v>315</v>
       </c>
       <c r="X17" s="312"/>
       <c r="Y17" s="183"/>
@@ -51972,7 +53163,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s" s="255">
-        <v>155</v>
+        <v>293</v>
       </c>
       <c r="C19" s="256"/>
       <c r="D19" s="256"/>
@@ -51995,7 +53186,7 @@
       <c r="S19" s="243"/>
       <c r="T19" s="243"/>
       <c r="U19" t="s" s="243">
-        <v>123</v>
+        <v>292</v>
       </c>
       <c r="V19" s="243"/>
       <c r="W19" s="243"/>
@@ -52078,7 +53269,7 @@
       <c r="C22" s="263"/>
       <c r="D22" s="263"/>
       <c r="E22" t="s" s="251">
-        <v>163</v>
+        <v>294</v>
       </c>
       <c r="F22" s="252"/>
       <c r="G22" s="252"/>
@@ -52106,7 +53297,7 @@
     </row>
     <row r="23" spans="1:28" s="179" customFormat="1" ht="18" customHeight="1">
       <c r="A23" t="s" s="307">
-        <v>199</v>
+        <v>311</v>
       </c>
       <c r="B23" s="307"/>
       <c r="C23" s="307"/>

</xml_diff>

<commit_message>
Process place and customerRefNumber fields of sample sheet
- Add new fields to API endpoints
- Parse new fields from excel sheet
- Write new fields to excel sheet and pdf sheet
- fixed writing empty comma to city/zip field if only one part of place is given

Ticket: mibi-portal-client#324, mibi-portal-client#326
Change-Id: I06d2f5b8b906e82ee5fddfd05e8d5c3835d02ca4
</commit_message>
<xml_diff>
--- a/test/data/mps155_timezone_bug_validated.xlsx
+++ b/test/data/mps155_timezone_bug_validated.xlsx
@@ -1705,9 +1705,6 @@
       </rPr>
       <t>d</t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">, </t>
   </si>
   <si>
     <r>
@@ -10001,7 +9998,9 @@
       <c r="Q6" t="s" s="143">
         <v>34</v>
       </c>
-      <c r="R6" s="219"/>
+      <c r="R6" t="s" s="219">
+        <v>209</v>
+      </c>
       <c r="S6" s="220"/>
       <c r="T6" t="s" s="130">
         <v>77</v>
@@ -10349,7 +10348,7 @@
       </c>
       <c r="B19" s="220"/>
       <c r="C19" t="s" s="227">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D19" s="227"/>
       <c r="E19" s="227"/>
@@ -10476,7 +10475,7 @@
       <c r="H23" s="140"/>
       <c r="I23" s="140"/>
       <c r="J23" t="s" s="228">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K23" s="229"/>
       <c r="L23" s="229"/>
@@ -10556,7 +10555,9 @@
       <c r="S26" s="153"/>
     </row>
     <row r="27" spans="1:20" s="129" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="219"/>
+      <c r="A27" t="s" s="219">
+        <v>209</v>
+      </c>
       <c r="B27" s="220"/>
       <c r="C27" s="220"/>
       <c r="D27" s="220"/>
@@ -10755,7 +10756,7 @@
     </row>
     <row r="36" spans="1:25" s="127" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A36" t="s" s="146">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="140"/>
       <c r="C36" s="140"/>
@@ -10880,10 +10881,10 @@
         <v>53</v>
       </c>
       <c r="C41" t="s" s="111">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D41" t="s" s="112">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E41" t="s" s="113">
         <v>73</v>
@@ -10892,69 +10893,69 @@
         <v>1</v>
       </c>
       <c r="G41" t="s" s="111">
+        <v>216</v>
+      </c>
+      <c r="H41" t="s" s="115">
         <v>217</v>
       </c>
-      <c r="H41" t="s" s="115">
+      <c r="I41" t="s" s="112">
         <v>218</v>
       </c>
-      <c r="I41" t="s" s="112">
+      <c r="J41" t="s" s="113">
         <v>219</v>
       </c>
-      <c r="J41" t="s" s="113">
+      <c r="K41" t="s" s="115">
         <v>220</v>
       </c>
-      <c r="K41" t="s" s="115">
+      <c r="L41" t="s" s="114">
         <v>221</v>
       </c>
-      <c r="L41" t="s" s="114">
+      <c r="M41" t="s" s="116">
         <v>222</v>
       </c>
-      <c r="M41" t="s" s="116">
+      <c r="N41" t="s" s="113">
         <v>223</v>
       </c>
-      <c r="N41" t="s" s="113">
+      <c r="O41" t="s" s="114">
         <v>224</v>
       </c>
-      <c r="O41" t="s" s="114">
+      <c r="P41" t="s" s="111">
         <v>225</v>
       </c>
-      <c r="P41" t="s" s="111">
+      <c r="Q41" t="s" s="112">
         <v>226</v>
-      </c>
-      <c r="Q41" t="s" s="112">
-        <v>227</v>
       </c>
       <c r="R41" t="s" s="116">
         <v>144</v>
       </c>
       <c r="S41" t="s" s="116">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" s="77" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A42" t="s" s="315">
         <v>228</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" s="77" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A42" t="s" s="315">
+      <c r="B42" t="s" s="316">
         <v>229</v>
       </c>
-      <c r="B42" t="s" s="316">
+      <c r="C42" t="s" s="317">
         <v>230</v>
-      </c>
-      <c r="C42" t="s" s="317">
-        <v>231</v>
       </c>
       <c r="D42" t="s" s="318">
         <v>209</v>
       </c>
       <c r="E42" t="s" s="319">
+        <v>231</v>
+      </c>
+      <c r="F42" t="s" s="320">
         <v>232</v>
       </c>
-      <c r="F42" t="s" s="320">
+      <c r="G42" t="s" s="321">
         <v>233</v>
       </c>
-      <c r="G42" t="s" s="321">
+      <c r="H42" t="s" s="322">
         <v>234</v>
-      </c>
-      <c r="H42" t="s" s="322">
-        <v>235</v>
       </c>
       <c r="I42" t="s" s="323">
         <v>54</v>
@@ -10963,25 +10964,25 @@
         <v>89</v>
       </c>
       <c r="K42" t="s" s="325">
+        <v>235</v>
+      </c>
+      <c r="L42" t="s" s="326">
         <v>236</v>
       </c>
-      <c r="L42" t="s" s="326">
+      <c r="M42" t="s" s="327">
         <v>237</v>
       </c>
-      <c r="M42" t="s" s="327">
+      <c r="N42" t="s" s="328">
         <v>238</v>
       </c>
-      <c r="N42" t="s" s="328">
+      <c r="O42" t="s" s="329">
         <v>239</v>
       </c>
-      <c r="O42" t="s" s="329">
+      <c r="P42" t="s" s="330">
         <v>240</v>
       </c>
-      <c r="P42" t="s" s="330">
+      <c r="Q42" t="s" s="331">
         <v>241</v>
-      </c>
-      <c r="Q42" t="s" s="331">
-        <v>242</v>
       </c>
       <c r="R42" t="s" s="332">
         <v>209</v>
@@ -10999,22 +11000,22 @@
         <v>209</v>
       </c>
       <c r="C43" t="s" s="337">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D43" t="s" s="338">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E43" t="s" s="339">
+        <v>232</v>
+      </c>
+      <c r="F43" t="s" s="340">
+        <v>242</v>
+      </c>
+      <c r="G43" t="s" s="341">
         <v>233</v>
       </c>
-      <c r="F43" t="s" s="340">
-        <v>243</v>
-      </c>
-      <c r="G43" t="s" s="341">
+      <c r="H43" t="s" s="342">
         <v>234</v>
-      </c>
-      <c r="H43" t="s" s="342">
-        <v>235</v>
       </c>
       <c r="I43" t="s" s="343">
         <v>54</v>
@@ -11023,25 +11024,25 @@
         <v>89</v>
       </c>
       <c r="K43" t="s" s="345">
+        <v>235</v>
+      </c>
+      <c r="L43" t="s" s="346">
         <v>236</v>
       </c>
-      <c r="L43" t="s" s="346">
-        <v>237</v>
-      </c>
       <c r="M43" t="s" s="347">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N43" t="s" s="348">
+        <v>238</v>
+      </c>
+      <c r="O43" t="s" s="349">
         <v>239</v>
       </c>
-      <c r="O43" t="s" s="349">
+      <c r="P43" t="s" s="350">
         <v>240</v>
       </c>
-      <c r="P43" t="s" s="350">
+      <c r="Q43" t="s" s="351">
         <v>241</v>
-      </c>
-      <c r="Q43" t="s" s="351">
-        <v>242</v>
       </c>
       <c r="R43" t="s" s="352">
         <v>209</v>
@@ -11053,40 +11054,40 @@
     </row>
     <row r="44" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
       <c r="A44" t="s" s="355">
+        <v>244</v>
+      </c>
+      <c r="B44" t="s" s="356">
         <v>245</v>
       </c>
-      <c r="B44" t="s" s="356">
+      <c r="C44" t="s" s="357">
         <v>246</v>
-      </c>
-      <c r="C44" t="s" s="357">
-        <v>247</v>
       </c>
       <c r="D44" t="s" s="358">
         <v>209</v>
       </c>
       <c r="E44" t="s" s="359">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F44" t="s" s="360">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G44" t="s" s="361">
         <v>209</v>
       </c>
       <c r="H44" t="s" s="362">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I44" t="s" s="363">
         <v>54</v>
       </c>
       <c r="J44" t="s" s="364">
+        <v>249</v>
+      </c>
+      <c r="K44" t="s" s="365">
         <v>250</v>
       </c>
-      <c r="K44" t="s" s="365">
+      <c r="L44" t="s" s="366">
         <v>251</v>
-      </c>
-      <c r="L44" t="s" s="366">
-        <v>252</v>
       </c>
       <c r="M44" t="s" s="367">
         <v>209</v>
@@ -11098,43 +11099,43 @@
         <v>124</v>
       </c>
       <c r="P44" t="s" s="370">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q44" t="s" s="371">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R44" t="s" s="372">
         <v>209</v>
       </c>
       <c r="S44" t="s" s="373">
+        <v>254</v>
+      </c>
+      <c r="T44" s="374"/>
+    </row>
+    <row r="45" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A45" t="s" s="375">
         <v>255</v>
       </c>
-      <c r="T44" s="374"/>
-    </row>
-    <row r="45" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A45" t="s" s="375">
+      <c r="B45" t="s" s="376">
         <v>256</v>
       </c>
-      <c r="B45" t="s" s="376">
+      <c r="C45" t="s" s="377">
         <v>257</v>
-      </c>
-      <c r="C45" t="s" s="377">
-        <v>258</v>
       </c>
       <c r="D45" t="s" s="378">
         <v>209</v>
       </c>
       <c r="E45" t="s" s="379">
+        <v>258</v>
+      </c>
+      <c r="F45" t="s" s="380">
         <v>259</v>
       </c>
-      <c r="F45" t="s" s="380">
-        <v>260</v>
-      </c>
       <c r="G45" t="s" s="381">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H45" t="s" s="382">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I45" t="s" s="383">
         <v>54</v>
@@ -11143,202 +11144,202 @@
         <v>89</v>
       </c>
       <c r="K45" t="s" s="385">
+        <v>260</v>
+      </c>
+      <c r="L45" t="s" s="386">
         <v>261</v>
       </c>
-      <c r="L45" t="s" s="386">
-        <v>262</v>
-      </c>
       <c r="M45" t="s" s="387">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N45" t="s" s="388">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O45" t="s" s="389">
         <v>209</v>
       </c>
       <c r="P45" t="s" s="390">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q45" t="s" s="391">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="R45" t="s" s="392">
         <v>209</v>
       </c>
       <c r="S45" t="s" s="393">
+        <v>263</v>
+      </c>
+      <c r="T45" s="394"/>
+    </row>
+    <row r="46" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A46" t="s" s="395">
         <v>264</v>
       </c>
-      <c r="T45" s="394"/>
-    </row>
-    <row r="46" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A46" t="s" s="395">
+      <c r="B46" t="s" s="396">
         <v>265</v>
       </c>
-      <c r="B46" t="s" s="396">
-        <v>266</v>
-      </c>
       <c r="C46" t="s" s="397">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D46" t="s" s="398">
         <v>209</v>
       </c>
       <c r="E46" t="s" s="399">
+        <v>266</v>
+      </c>
+      <c r="F46" t="s" s="400">
         <v>267</v>
       </c>
-      <c r="F46" t="s" s="400">
-        <v>268</v>
-      </c>
       <c r="G46" t="s" s="401">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H46" t="s" s="402">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I46" t="s" s="403">
         <v>54</v>
       </c>
       <c r="J46" t="s" s="404">
+        <v>249</v>
+      </c>
+      <c r="K46" t="s" s="405">
         <v>250</v>
       </c>
-      <c r="K46" t="s" s="405">
+      <c r="L46" t="s" s="406">
         <v>251</v>
-      </c>
-      <c r="L46" t="s" s="406">
-        <v>252</v>
       </c>
       <c r="M46" t="s" s="407">
         <v>209</v>
       </c>
       <c r="N46" t="s" s="408">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O46" t="s" s="409">
         <v>124</v>
       </c>
       <c r="P46" t="s" s="410">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q46" t="s" s="411">
         <v>209</v>
       </c>
       <c r="R46" t="s" s="412">
+        <v>270</v>
+      </c>
+      <c r="S46" t="s" s="413">
+        <v>254</v>
+      </c>
+      <c r="T46" s="414"/>
+    </row>
+    <row r="47" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A47" t="s" s="415">
         <v>271</v>
       </c>
-      <c r="S46" t="s" s="413">
-        <v>255</v>
-      </c>
-      <c r="T46" s="414"/>
-    </row>
-    <row r="47" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A47" t="s" s="415">
+      <c r="B47" t="s" s="416">
         <v>272</v>
       </c>
-      <c r="B47" t="s" s="416">
-        <v>273</v>
-      </c>
       <c r="C47" t="s" s="417">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D47" t="s" s="418">
         <v>209</v>
       </c>
       <c r="E47" t="s" s="419">
+        <v>273</v>
+      </c>
+      <c r="F47" t="s" s="420">
         <v>274</v>
       </c>
-      <c r="F47" t="s" s="420">
-        <v>275</v>
-      </c>
       <c r="G47" t="s" s="421">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H47" t="s" s="422">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I47" t="s" s="423">
         <v>54</v>
       </c>
       <c r="J47" t="s" s="424">
+        <v>249</v>
+      </c>
+      <c r="K47" t="s" s="425">
         <v>250</v>
       </c>
-      <c r="K47" t="s" s="425">
+      <c r="L47" t="s" s="426">
         <v>251</v>
-      </c>
-      <c r="L47" t="s" s="426">
-        <v>252</v>
       </c>
       <c r="M47" t="s" s="427">
         <v>209</v>
       </c>
       <c r="N47" t="s" s="428">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O47" t="s" s="429">
         <v>124</v>
       </c>
       <c r="P47" t="s" s="430">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q47" t="s" s="431">
         <v>209</v>
       </c>
       <c r="R47" t="s" s="432">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S47" t="s" s="433">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="T47" s="434"/>
     </row>
     <row r="48" spans="1:25" s="11" customFormat="1" ht="21.75" customHeight="1">
       <c r="A48" t="s" s="435">
+        <v>275</v>
+      </c>
+      <c r="B48" t="s" s="436">
         <v>276</v>
       </c>
-      <c r="B48" t="s" s="436">
+      <c r="C48" t="s" s="437">
         <v>277</v>
-      </c>
-      <c r="C48" t="s" s="437">
-        <v>278</v>
       </c>
       <c r="D48" t="s" s="438">
         <v>209</v>
       </c>
       <c r="E48" t="s" s="439">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F48" t="s" s="440">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G48" t="s" s="441">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H48" t="s" s="442">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I48" t="s" s="443">
         <v>54</v>
       </c>
       <c r="J48" t="s" s="444">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K48" t="s" s="445">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="L48" t="s" s="446">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M48" t="s" s="447">
         <v>209</v>
       </c>
       <c r="N48" t="s" s="448">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O48" t="s" s="449">
         <v>209</v>
       </c>
       <c r="P48" t="s" s="450">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q48" t="s" s="451">
         <v>209</v>
@@ -51304,7 +51305,7 @@
       <c r="C6" s="256"/>
       <c r="D6" s="256"/>
       <c r="E6" t="s" s="257">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F6" s="258"/>
       <c r="G6" s="258"/>
@@ -51451,7 +51452,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s" s="255">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C11" s="256"/>
       <c r="D11" s="256"/>
@@ -51472,7 +51473,7 @@
       <c r="Q11" s="243"/>
       <c r="R11" s="243"/>
       <c r="S11" t="s" s="243">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T11" s="244"/>
     </row>
@@ -51537,7 +51538,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s" s="268">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="256"/>
       <c r="D14" s="256"/>
@@ -51556,11 +51557,11 @@
       <c r="O14" s="258"/>
       <c r="P14" s="259"/>
       <c r="Q14" t="s" s="243">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R14" s="243"/>
       <c r="S14" t="s" s="243">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T14" s="244"/>
     </row>
@@ -51569,7 +51570,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s" s="255">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C15" s="256"/>
       <c r="D15" s="256"/>
@@ -51625,12 +51626,12 @@
         <v>25</v>
       </c>
       <c r="B17" t="s" s="255">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C17" s="255"/>
       <c r="D17" s="255"/>
       <c r="E17" t="s" s="257">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F17" s="258"/>
       <c r="G17" s="258"/>
@@ -51646,7 +51647,7 @@
       <c r="Q17" s="243"/>
       <c r="R17" s="243"/>
       <c r="S17" t="s" s="243">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T17" s="244"/>
     </row>
@@ -51655,7 +51656,7 @@
         <v>61</v>
       </c>
       <c r="B18" t="s" s="255">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="256"/>
       <c r="D18" s="256"/>
@@ -51676,7 +51677,7 @@
       <c r="Q18" s="243"/>
       <c r="R18" s="243"/>
       <c r="S18" t="s" s="243">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T18" s="244"/>
     </row>
@@ -51713,7 +51714,7 @@
         <v>63</v>
       </c>
       <c r="B20" t="s" s="255">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20" s="256"/>
       <c r="D20" s="256"/>
@@ -51734,7 +51735,7 @@
       <c r="Q20" s="243"/>
       <c r="R20" s="243"/>
       <c r="S20" t="s" s="243">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T20" s="244"/>
     </row>
@@ -51792,7 +51793,7 @@
       <c r="Q22" s="243"/>
       <c r="R22" s="243"/>
       <c r="S22" t="s" s="243">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T22" s="244"/>
     </row>
@@ -51806,7 +51807,7 @@
       <c r="C23" s="263"/>
       <c r="D23" s="263"/>
       <c r="E23" t="s" s="251">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F23" s="252"/>
       <c r="G23" s="252"/>
@@ -51951,10 +51952,10 @@
         <v>53</v>
       </c>
       <c r="D29" t="s" s="27">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E29" t="s" s="28">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F29" t="s" s="7">
         <v>73</v>
@@ -51963,43 +51964,43 @@
         <v>1</v>
       </c>
       <c r="H29" t="s" s="27">
+        <v>296</v>
+      </c>
+      <c r="I29" t="s" s="8">
         <v>297</v>
       </c>
-      <c r="I29" t="s" s="8">
+      <c r="J29" t="s" s="28">
         <v>298</v>
       </c>
-      <c r="J29" t="s" s="28">
+      <c r="K29" t="s" s="7">
         <v>299</v>
       </c>
-      <c r="K29" t="s" s="7">
+      <c r="L29" t="s" s="8">
         <v>300</v>
       </c>
-      <c r="L29" t="s" s="8">
+      <c r="M29" t="s" s="9">
         <v>301</v>
       </c>
-      <c r="M29" t="s" s="9">
+      <c r="N29" t="s" s="29">
         <v>302</v>
       </c>
-      <c r="N29" t="s" s="29">
+      <c r="O29" t="s" s="7">
         <v>303</v>
       </c>
-      <c r="O29" t="s" s="7">
+      <c r="P29" t="s" s="9">
         <v>304</v>
       </c>
-      <c r="P29" t="s" s="9">
+      <c r="Q29" t="s" s="27">
         <v>305</v>
       </c>
-      <c r="Q29" t="s" s="27">
+      <c r="R29" t="s" s="28">
         <v>306</v>
-      </c>
-      <c r="R29" t="s" s="28">
-        <v>307</v>
       </c>
       <c r="S29" t="s" s="31">
         <v>96</v>
       </c>
       <c r="T29" t="s" s="30">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="33.75">
@@ -52230,7 +52231,7 @@
     </row>
     <row r="36" spans="1:20" s="72" customFormat="1" ht="24.75" customHeight="1">
       <c r="A36" t="s" s="254">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B36" s="254"/>
       <c r="C36" s="254"/>
@@ -52254,7 +52255,7 @@
     </row>
     <row r="37" spans="1:20" s="72" customFormat="1" ht="12.95" customHeight="1">
       <c r="A37" t="s" s="248">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B37" s="248"/>
       <c r="C37" s="248"/>
@@ -52350,7 +52351,7 @@
     </row>
     <row r="41" spans="1:20" s="72" customFormat="1" ht="12.95" customHeight="1">
       <c r="A41" t="s" s="248">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B41" s="248"/>
       <c r="C41" s="248"/>
@@ -52604,7 +52605,7 @@
       </c>
       <c r="R3" s="284"/>
       <c r="S3" t="s" s="280">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T3" s="284"/>
       <c r="U3" t="s" s="301">
@@ -52668,7 +52669,7 @@
       <c r="C5" s="256"/>
       <c r="D5" s="256"/>
       <c r="E5" t="s" s="257">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F5" s="258"/>
       <c r="G5" s="258"/>
@@ -52729,7 +52730,7 @@
       </c>
       <c r="V6" s="243"/>
       <c r="W6" t="s" s="297">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="X6" s="304"/>
       <c r="Y6" s="183"/>
@@ -52846,7 +52847,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s" s="255">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C10" s="256"/>
       <c r="D10" s="256"/>
@@ -52867,11 +52868,11 @@
       <c r="Q10" s="243"/>
       <c r="R10" s="243"/>
       <c r="S10" t="s" s="243">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T10" s="243"/>
       <c r="U10" t="s" s="243">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="V10" s="243"/>
       <c r="W10" s="243"/>
@@ -52949,7 +52950,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s" s="268">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C13" s="256"/>
       <c r="D13" s="256"/>
@@ -52968,19 +52969,19 @@
       <c r="O13" s="258"/>
       <c r="P13" s="259"/>
       <c r="Q13" t="s" s="243">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R13" s="243"/>
       <c r="S13" t="s" s="243">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T13" s="243"/>
       <c r="U13" t="s" s="243">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="V13" s="243"/>
       <c r="W13" t="s" s="243">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="X13" s="244"/>
       <c r="Y13" s="183"/>
@@ -52990,7 +52991,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s" s="255">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C14" s="256"/>
       <c r="D14" s="256"/>
@@ -53056,7 +53057,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s" s="255">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C16" s="255"/>
       <c r="D16" s="255"/>
@@ -53089,7 +53090,7 @@
         <v>61</v>
       </c>
       <c r="B17" t="s" s="255">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C17" s="256"/>
       <c r="D17" s="256"/>
@@ -53108,19 +53109,19 @@
       <c r="O17" s="258"/>
       <c r="P17" s="259"/>
       <c r="Q17" t="s" s="297">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="R17" s="298"/>
       <c r="S17" t="s" s="243">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T17" s="243"/>
       <c r="U17" t="s" s="243">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="V17" s="243"/>
       <c r="W17" t="s" s="297">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="X17" s="312"/>
       <c r="Y17" s="183"/>
@@ -53163,7 +53164,7 @@
         <v>63</v>
       </c>
       <c r="B19" t="s" s="255">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C19" s="256"/>
       <c r="D19" s="256"/>
@@ -53186,7 +53187,7 @@
       <c r="S19" s="243"/>
       <c r="T19" s="243"/>
       <c r="U19" t="s" s="243">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="V19" s="243"/>
       <c r="W19" s="243"/>
@@ -53269,7 +53270,7 @@
       <c r="C22" s="263"/>
       <c r="D22" s="263"/>
       <c r="E22" t="s" s="251">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F22" s="252"/>
       <c r="G22" s="252"/>
@@ -53297,7 +53298,7 @@
     </row>
     <row r="23" spans="1:28" s="179" customFormat="1" ht="18" customHeight="1">
       <c r="A23" t="s" s="307">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B23" s="307"/>
       <c r="C23" s="307"/>

</xml_diff>